<commit_message>
basic functions for import and adding of chrons
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -78,13 +78,13 @@
     <t>sub</t>
   </si>
   <si>
-    <t>comp</t>
-  </si>
-  <si>
     <t>column_tot</t>
   </si>
   <si>
     <t>Start</t>
+  </si>
+  <si>
+    <t>add</t>
   </si>
 </sst>
 </file>
@@ -419,10 +419,10 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -432,7 +432,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -441,7 +441,7 @@
         <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G1" t="s">
         <v>18</v>
@@ -553,7 +553,7 @@
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -576,7 +576,7 @@
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -599,7 +599,7 @@
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -622,7 +622,7 @@
         <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -857,7 +857,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -870,7 +870,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>